<commit_message>
Postgres SQL analysis files added to the project
</commit_message>
<xml_diff>
--- a/tfl_time_table_ex/London_tube_lines v2.xlsx
+++ b/tfl_time_table_ex/London_tube_lines v2.xlsx
@@ -5,28 +5,28 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucesnsa\PycharmProjects\transport_risk_profile\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucesnsa\PycharmProjects\transport_risk_profile\tfl_time_table_ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="773"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="773" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="WC" sheetId="11" r:id="rId1"/>
-    <sheet name="bakerloo" sheetId="1" r:id="rId2"/>
-    <sheet name="central" sheetId="2" r:id="rId3"/>
-    <sheet name="circle" sheetId="3" r:id="rId4"/>
-    <sheet name="district" sheetId="4" r:id="rId5"/>
+    <sheet name="Bakerloo" sheetId="1" r:id="rId2"/>
+    <sheet name="Central" sheetId="2" r:id="rId3"/>
+    <sheet name="Circle" sheetId="3" r:id="rId4"/>
+    <sheet name="District" sheetId="4" r:id="rId5"/>
     <sheet name="HammersmithCity" sheetId="5" r:id="rId6"/>
     <sheet name="Jubilee" sheetId="6" r:id="rId7"/>
     <sheet name="Metropolitan" sheetId="7" r:id="rId8"/>
     <sheet name="Northern" sheetId="8" r:id="rId9"/>
     <sheet name="Piccadilly" sheetId="9" r:id="rId10"/>
     <sheet name="Victoria" sheetId="10" r:id="rId11"/>
-    <sheet name="LondonOverground" sheetId="14" r:id="rId12"/>
+    <sheet name="Overground" sheetId="14" r:id="rId12"/>
     <sheet name="DLR" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="152511" iterateCount="200"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1288,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3283,7 +3283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>